<commit_message>
2 commit Changes are: layout,about,contact,navbar,portfolio
</commit_message>
<xml_diff>
--- a/public/contacts.xlsx
+++ b/public/contacts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>First Name</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>ksanu@gmail.com</t>
+  </si>
+  <si>
+    <t>sid</t>
+  </si>
+  <si>
+    <t>kmr</t>
+  </si>
+  <si>
+    <t>sid1235@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -407,7 +416,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -499,6 +508,17 @@
         <v>16</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>